<commit_message>
GUI done 0.2 + xlsx uploa
</commit_message>
<xml_diff>
--- a/project_db_test_publish.xlsx
+++ b/project_db_test_publish.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayeletgoldstein/Dropbox/Hadassah College/Courses/AI in Medicine/בינה מלאכותית ברפואה _ MDSS_18/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvir levi\PycharmProjects\CDSS-Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B252714A-A852-CB46-A633-0E315946D16E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4C3F0E-4BF6-4058-B448-1F57C58C089E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="1160" windowWidth="22760" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -576,23 +576,23 @@
   <dimension ref="A1:J271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" style="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="7" max="7" width="18.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -616,7 +616,7 @@
       </c>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
@@ -640,7 +640,7 @@
       </c>
       <c r="H2" s="6"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>28</v>
       </c>
@@ -666,7 +666,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -692,7 +692,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -718,7 +718,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -744,7 +744,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
@@ -770,7 +770,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -796,7 +796,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -848,7 +848,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -874,7 +874,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
@@ -900,7 +900,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -926,7 +926,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -978,7 +978,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -1004,7 +1004,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1030,7 +1030,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>33</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1082,7 +1082,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
@@ -1108,7 +1108,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1186,7 +1186,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -1212,7 +1212,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
@@ -1238,7 +1238,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
@@ -1264,7 +1264,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1290,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1316,7 +1316,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1342,7 +1342,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>28</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>28</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>32</v>
       </c>
@@ -1498,7 +1498,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>32</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>32</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>32</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -1602,7 +1602,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -1628,7 +1628,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>31</v>
       </c>
@@ -1680,7 +1680,7 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>31</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>31</v>
       </c>
@@ -1732,7 +1732,7 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -1758,7 +1758,7 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
@@ -1784,7 +1784,7 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>33</v>
       </c>
@@ -1836,7 +1836,7 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>33</v>
       </c>
@@ -1862,7 +1862,7 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
@@ -1888,7 +1888,7 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>28</v>
       </c>
@@ -1914,7 +1914,7 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>28</v>
       </c>
@@ -1940,7 +1940,7 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>28</v>
       </c>
@@ -1966,7 +1966,7 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>28</v>
       </c>
@@ -1992,7 +1992,7 @@
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
     </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>32</v>
       </c>
@@ -2018,7 +2018,7 @@
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
     </row>
-    <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>32</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
     </row>
-    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>32</v>
       </c>
@@ -2070,7 +2070,7 @@
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
     </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>31</v>
       </c>
@@ -2096,7 +2096,7 @@
       <c r="I58" s="5"/>
       <c r="J58" s="5"/>
     </row>
-    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>31</v>
       </c>
@@ -2122,7 +2122,7 @@
       <c r="I59" s="5"/>
       <c r="J59" s="5"/>
     </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>31</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
     </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>31</v>
       </c>
@@ -2174,7 +2174,7 @@
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>28</v>
       </c>
@@ -2200,7 +2200,7 @@
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>31</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>32</v>
       </c>
@@ -2252,7 +2252,7 @@
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>7</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>32</v>
       </c>
@@ -2304,7 +2304,7 @@
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>32</v>
       </c>
@@ -2330,7 +2330,7 @@
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>32</v>
       </c>
@@ -2356,7 +2356,7 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>32</v>
       </c>
@@ -2382,7 +2382,7 @@
       <c r="I69" s="5"/>
       <c r="J69" s="5"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>32</v>
       </c>
@@ -2408,7 +2408,7 @@
       <c r="I70" s="5"/>
       <c r="J70" s="5"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>32</v>
       </c>
@@ -2434,7 +2434,7 @@
       <c r="I71" s="5"/>
       <c r="J71" s="5"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>32</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>32</v>
       </c>
@@ -2486,7 +2486,7 @@
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
     </row>
-    <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>33</v>
       </c>
@@ -2512,7 +2512,7 @@
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
     </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>33</v>
       </c>
@@ -2538,7 +2538,7 @@
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
     </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>33</v>
       </c>
@@ -2564,7 +2564,7 @@
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
     </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>33</v>
       </c>
@@ -2590,7 +2590,7 @@
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
     </row>
-    <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>33</v>
       </c>
@@ -2616,7 +2616,7 @@
       <c r="I78" s="5"/>
       <c r="J78" s="5"/>
     </row>
-    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>28</v>
       </c>
@@ -2642,7 +2642,7 @@
       <c r="I79" s="5"/>
       <c r="J79" s="5"/>
     </row>
-    <row r="80" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>28</v>
       </c>
@@ -2668,7 +2668,7 @@
       <c r="I80" s="5"/>
       <c r="J80" s="5"/>
     </row>
-    <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>28</v>
       </c>
@@ -2694,7 +2694,7 @@
       <c r="I81" s="5"/>
       <c r="J81" s="5"/>
     </row>
-    <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>32</v>
       </c>
@@ -2720,7 +2720,7 @@
       <c r="I82" s="5"/>
       <c r="J82" s="5"/>
     </row>
-    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>32</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>
     </row>
-    <row r="84" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>32</v>
       </c>
@@ -2772,7 +2772,7 @@
       <c r="I84" s="5"/>
       <c r="J84" s="5"/>
     </row>
-    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>32</v>
       </c>
@@ -2798,7 +2798,7 @@
       <c r="I85" s="5"/>
       <c r="J85" s="5"/>
     </row>
-    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>31</v>
       </c>
@@ -2824,7 +2824,7 @@
       <c r="I86" s="5"/>
       <c r="J86" s="5"/>
     </row>
-    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>31</v>
       </c>
@@ -2850,7 +2850,7 @@
       <c r="I87" s="5"/>
       <c r="J87" s="5"/>
     </row>
-    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>31</v>
       </c>
@@ -2876,7 +2876,7 @@
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
     </row>
-    <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>31</v>
       </c>
@@ -2902,7 +2902,7 @@
       <c r="I89" s="5"/>
       <c r="J89" s="5"/>
     </row>
-    <row r="90" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>31</v>
       </c>
@@ -2928,7 +2928,7 @@
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
     </row>
-    <row r="91" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>31</v>
       </c>
@@ -2954,7 +2954,7 @@
       <c r="I91" s="5"/>
       <c r="J91" s="5"/>
     </row>
-    <row r="92" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>31</v>
       </c>
@@ -2980,7 +2980,7 @@
       <c r="I92" s="5"/>
       <c r="J92" s="5"/>
     </row>
-    <row r="93" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>31</v>
       </c>
@@ -3006,7 +3006,7 @@
       <c r="I93" s="5"/>
       <c r="J93" s="5"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>32</v>
       </c>
@@ -3032,7 +3032,7 @@
       <c r="I94" s="5"/>
       <c r="J94" s="5"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>32</v>
       </c>
@@ -3058,7 +3058,7 @@
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>32</v>
       </c>
@@ -3084,7 +3084,7 @@
       <c r="I96" s="5"/>
       <c r="J96" s="5"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>32</v>
       </c>
@@ -3110,7 +3110,7 @@
       <c r="I97" s="5"/>
       <c r="J97" s="5"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>32</v>
       </c>
@@ -3136,7 +3136,7 @@
       <c r="I98" s="5"/>
       <c r="J98" s="5"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>32</v>
       </c>
@@ -3162,7 +3162,7 @@
       <c r="I99" s="5"/>
       <c r="J99" s="5"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>32</v>
       </c>
@@ -3188,7 +3188,7 @@
       <c r="I100" s="5"/>
       <c r="J100" s="5"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>32</v>
       </c>
@@ -3214,7 +3214,7 @@
       <c r="I101" s="5"/>
       <c r="J101" s="5"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>32</v>
       </c>
@@ -3240,7 +3240,7 @@
       <c r="I102" s="5"/>
       <c r="J102" s="5"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>32</v>
       </c>
@@ -3266,7 +3266,7 @@
       <c r="I103" s="5"/>
       <c r="J103" s="5"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>32</v>
       </c>
@@ -3292,7 +3292,7 @@
       <c r="I104" s="5"/>
       <c r="J104" s="5"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>32</v>
       </c>
@@ -3318,7 +3318,7 @@
       <c r="I105" s="5"/>
       <c r="J105" s="5"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>28</v>
       </c>
@@ -3344,7 +3344,7 @@
       <c r="I106" s="5"/>
       <c r="J106" s="5"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>32</v>
       </c>
@@ -3370,7 +3370,7 @@
       <c r="I107" s="5"/>
       <c r="J107" s="5"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>28</v>
       </c>
@@ -3396,7 +3396,7 @@
       <c r="I108" s="5"/>
       <c r="J108" s="5"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>31</v>
       </c>
@@ -3422,7 +3422,7 @@
       <c r="I109" s="5"/>
       <c r="J109" s="5"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>33</v>
       </c>
@@ -3448,7 +3448,7 @@
       <c r="I110" s="5"/>
       <c r="J110" s="5"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>28</v>
       </c>
@@ -3474,7 +3474,7 @@
       <c r="I111" s="5"/>
       <c r="J111" s="5"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>28</v>
       </c>
@@ -3500,7 +3500,7 @@
       <c r="I112" s="5"/>
       <c r="J112" s="5"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>32</v>
       </c>
@@ -3526,7 +3526,7 @@
       <c r="I113" s="5"/>
       <c r="J113" s="5"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>33</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="I114" s="5"/>
       <c r="J114" s="5"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>31</v>
       </c>
@@ -3578,7 +3578,7 @@
       <c r="I115" s="5"/>
       <c r="J115" s="5"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>32</v>
       </c>
@@ -3604,7 +3604,7 @@
       <c r="I116" s="5"/>
       <c r="J116" s="5"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>33</v>
       </c>
@@ -3630,7 +3630,7 @@
       <c r="I117" s="5"/>
       <c r="J117" s="5"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>28</v>
       </c>
@@ -3656,7 +3656,7 @@
       <c r="I118" s="5"/>
       <c r="J118" s="5"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>28</v>
       </c>
@@ -3682,7 +3682,7 @@
       <c r="I119" s="5"/>
       <c r="J119" s="5"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>7</v>
       </c>
@@ -3708,7 +3708,7 @@
       <c r="I120" s="5"/>
       <c r="J120" s="5"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>28</v>
       </c>
@@ -3734,7 +3734,7 @@
       <c r="I121" s="5"/>
       <c r="J121" s="5"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>33</v>
       </c>
@@ -3760,7 +3760,7 @@
       <c r="I122" s="5"/>
       <c r="J122" s="5"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>32</v>
       </c>
@@ -3786,7 +3786,7 @@
       <c r="I123" s="5"/>
       <c r="J123" s="5"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>28</v>
       </c>
@@ -3812,7 +3812,7 @@
       <c r="I124" s="5"/>
       <c r="J124" s="5"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>7</v>
       </c>
@@ -3838,7 +3838,7 @@
       <c r="I125" s="5"/>
       <c r="J125" s="5"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>33</v>
       </c>
@@ -3864,7 +3864,7 @@
       <c r="I126" s="5"/>
       <c r="J126" s="5"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>28</v>
       </c>
@@ -3890,7 +3890,7 @@
       <c r="I127" s="5"/>
       <c r="J127" s="5"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>28</v>
       </c>
@@ -3916,7 +3916,7 @@
       <c r="I128" s="5"/>
       <c r="J128" s="5"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>7</v>
       </c>
@@ -3942,7 +3942,7 @@
       <c r="I129" s="5"/>
       <c r="J129" s="5"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>33</v>
       </c>
@@ -3968,7 +3968,7 @@
       <c r="I130" s="5"/>
       <c r="J130" s="5"/>
     </row>
-    <row r="131" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>33</v>
       </c>
@@ -3994,7 +3994,7 @@
       <c r="I131" s="5"/>
       <c r="J131" s="5"/>
     </row>
-    <row r="132" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>33</v>
       </c>
@@ -4020,7 +4020,7 @@
       <c r="I132" s="5"/>
       <c r="J132" s="5"/>
     </row>
-    <row r="133" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>33</v>
       </c>
@@ -4046,7 +4046,7 @@
       <c r="I133" s="5"/>
       <c r="J133" s="5"/>
     </row>
-    <row r="134" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>33</v>
       </c>
@@ -4072,7 +4072,7 @@
       <c r="I134" s="5"/>
       <c r="J134" s="5"/>
     </row>
-    <row r="135" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>33</v>
       </c>
@@ -4098,7 +4098,7 @@
       <c r="I135" s="5"/>
       <c r="J135" s="5"/>
     </row>
-    <row r="136" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>33</v>
       </c>
@@ -4124,7 +4124,7 @@
       <c r="I136" s="5"/>
       <c r="J136" s="5"/>
     </row>
-    <row r="137" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>33</v>
       </c>
@@ -4150,7 +4150,7 @@
       <c r="I137" s="5"/>
       <c r="J137" s="5"/>
     </row>
-    <row r="138" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>33</v>
       </c>
@@ -4176,7 +4176,7 @@
       <c r="I138" s="5"/>
       <c r="J138" s="5"/>
     </row>
-    <row r="139" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>28</v>
       </c>
@@ -4202,7 +4202,7 @@
       <c r="I139" s="5"/>
       <c r="J139" s="5"/>
     </row>
-    <row r="140" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>28</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="I140" s="5"/>
       <c r="J140" s="5"/>
     </row>
-    <row r="141" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>28</v>
       </c>
@@ -4254,7 +4254,7 @@
       <c r="I141" s="5"/>
       <c r="J141" s="5"/>
     </row>
-    <row r="142" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>28</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="I142" s="5"/>
       <c r="J142" s="5"/>
     </row>
-    <row r="143" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>28</v>
       </c>
@@ -4306,7 +4306,7 @@
       <c r="I143" s="5"/>
       <c r="J143" s="5"/>
     </row>
-    <row r="144" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>28</v>
       </c>
@@ -4332,7 +4332,7 @@
       <c r="I144" s="5"/>
       <c r="J144" s="5"/>
     </row>
-    <row r="145" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>28</v>
       </c>
@@ -4358,7 +4358,7 @@
       <c r="I145" s="5"/>
       <c r="J145" s="5"/>
     </row>
-    <row r="146" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>28</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="I146" s="5"/>
       <c r="J146" s="5"/>
     </row>
-    <row r="147" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>28</v>
       </c>
@@ -4410,7 +4410,7 @@
       <c r="I147" s="5"/>
       <c r="J147" s="5"/>
     </row>
-    <row r="148" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>28</v>
       </c>
@@ -4436,7 +4436,7 @@
       <c r="I148" s="5"/>
       <c r="J148" s="5"/>
     </row>
-    <row r="149" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>28</v>
       </c>
@@ -4462,7 +4462,7 @@
       <c r="I149" s="5"/>
       <c r="J149" s="5"/>
     </row>
-    <row r="150" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>32</v>
       </c>
@@ -4488,7 +4488,7 @@
       <c r="I150" s="5"/>
       <c r="J150" s="5"/>
     </row>
-    <row r="151" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>32</v>
       </c>
@@ -4514,7 +4514,7 @@
       <c r="I151" s="5"/>
       <c r="J151" s="5"/>
     </row>
-    <row r="152" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>32</v>
       </c>
@@ -4540,7 +4540,7 @@
       <c r="I152" s="5"/>
       <c r="J152" s="5"/>
     </row>
-    <row r="153" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>32</v>
       </c>
@@ -4566,7 +4566,7 @@
       <c r="I153" s="5"/>
       <c r="J153" s="5"/>
     </row>
-    <row r="154" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A154" s="1" t="s">
         <v>32</v>
       </c>
@@ -4592,7 +4592,7 @@
       <c r="I154" s="5"/>
       <c r="J154" s="5"/>
     </row>
-    <row r="155" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A155" s="1" t="s">
         <v>32</v>
       </c>
@@ -4618,7 +4618,7 @@
       <c r="I155" s="5"/>
       <c r="J155" s="5"/>
     </row>
-    <row r="156" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A156" s="1" t="s">
         <v>32</v>
       </c>
@@ -4644,7 +4644,7 @@
       <c r="I156" s="5"/>
       <c r="J156" s="5"/>
     </row>
-    <row r="157" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>32</v>
       </c>
@@ -4670,7 +4670,7 @@
       <c r="I157" s="5"/>
       <c r="J157" s="5"/>
     </row>
-    <row r="158" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>32</v>
       </c>
@@ -4696,7 +4696,7 @@
       <c r="I158" s="5"/>
       <c r="J158" s="5"/>
     </row>
-    <row r="159" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>32</v>
       </c>
@@ -4722,7 +4722,7 @@
       <c r="I159" s="5"/>
       <c r="J159" s="5"/>
     </row>
-    <row r="160" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>32</v>
       </c>
@@ -4748,7 +4748,7 @@
       <c r="I160" s="5"/>
       <c r="J160" s="5"/>
     </row>
-    <row r="161" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>32</v>
       </c>
@@ -4774,7 +4774,7 @@
       <c r="I161" s="5"/>
       <c r="J161" s="5"/>
     </row>
-    <row r="162" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A162" s="1" t="s">
         <v>32</v>
       </c>
@@ -4800,7 +4800,7 @@
       <c r="I162" s="5"/>
       <c r="J162" s="5"/>
     </row>
-    <row r="163" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>32</v>
       </c>
@@ -4826,7 +4826,7 @@
       <c r="I163" s="5"/>
       <c r="J163" s="5"/>
     </row>
-    <row r="164" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A164" s="1" t="s">
         <v>32</v>
       </c>
@@ -4852,7 +4852,7 @@
       <c r="I164" s="5"/>
       <c r="J164" s="5"/>
     </row>
-    <row r="165" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A165" s="1" t="s">
         <v>31</v>
       </c>
@@ -4878,7 +4878,7 @@
       <c r="I165" s="5"/>
       <c r="J165" s="5"/>
     </row>
-    <row r="166" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A166" s="1" t="s">
         <v>31</v>
       </c>
@@ -4904,7 +4904,7 @@
       <c r="I166" s="5"/>
       <c r="J166" s="5"/>
     </row>
-    <row r="167" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A167" s="1" t="s">
         <v>31</v>
       </c>
@@ -4930,7 +4930,7 @@
       <c r="I167" s="5"/>
       <c r="J167" s="5"/>
     </row>
-    <row r="168" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A168" s="1" t="s">
         <v>31</v>
       </c>
@@ -4956,7 +4956,7 @@
       <c r="I168" s="5"/>
       <c r="J168" s="5"/>
     </row>
-    <row r="169" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A169" s="1" t="s">
         <v>31</v>
       </c>
@@ -4982,7 +4982,7 @@
       <c r="I169" s="5"/>
       <c r="J169" s="5"/>
     </row>
-    <row r="170" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A170" s="1" t="s">
         <v>31</v>
       </c>
@@ -5008,7 +5008,7 @@
       <c r="I170" s="5"/>
       <c r="J170" s="5"/>
     </row>
-    <row r="171" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A171" s="1" t="s">
         <v>31</v>
       </c>
@@ -5034,7 +5034,7 @@
       <c r="I171" s="5"/>
       <c r="J171" s="5"/>
     </row>
-    <row r="172" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A172" s="1" t="s">
         <v>31</v>
       </c>
@@ -5060,7 +5060,7 @@
       <c r="I172" s="5"/>
       <c r="J172" s="5"/>
     </row>
-    <row r="173" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A173" s="1" t="s">
         <v>31</v>
       </c>
@@ -5086,7 +5086,7 @@
       <c r="I173" s="5"/>
       <c r="J173" s="5"/>
     </row>
-    <row r="174" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A174" s="1" t="s">
         <v>31</v>
       </c>
@@ -5112,7 +5112,7 @@
       <c r="I174" s="5"/>
       <c r="J174" s="5"/>
     </row>
-    <row r="175" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A175" s="1" t="s">
         <v>31</v>
       </c>
@@ -5138,7 +5138,7 @@
       <c r="I175" s="5"/>
       <c r="J175" s="5"/>
     </row>
-    <row r="176" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A176" s="1" t="s">
         <v>31</v>
       </c>
@@ -5164,7 +5164,7 @@
       <c r="I176" s="5"/>
       <c r="J176" s="5"/>
     </row>
-    <row r="177" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A177" s="1" t="s">
         <v>31</v>
       </c>
@@ -5190,7 +5190,7 @@
       <c r="I177" s="5"/>
       <c r="J177" s="5"/>
     </row>
-    <row r="178" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>31</v>
       </c>
@@ -5216,7 +5216,7 @@
       <c r="I178" s="5"/>
       <c r="J178" s="5"/>
     </row>
-    <row r="179" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>31</v>
       </c>
@@ -5242,7 +5242,7 @@
       <c r="I179" s="5"/>
       <c r="J179" s="5"/>
     </row>
-    <row r="180" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>14</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="I180" s="5"/>
       <c r="J180" s="5"/>
     </row>
-    <row r="181" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>14</v>
       </c>
@@ -5294,7 +5294,7 @@
       <c r="I181" s="5"/>
       <c r="J181" s="5"/>
     </row>
-    <row r="182" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>14</v>
       </c>
@@ -5320,7 +5320,7 @@
       <c r="I182" s="5"/>
       <c r="J182" s="5"/>
     </row>
-    <row r="183" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>14</v>
       </c>
@@ -5346,7 +5346,7 @@
       <c r="I183" s="5"/>
       <c r="J183" s="5"/>
     </row>
-    <row r="184" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>14</v>
       </c>
@@ -5372,7 +5372,7 @@
       <c r="I184" s="5"/>
       <c r="J184" s="5"/>
     </row>
-    <row r="185" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>14</v>
       </c>
@@ -5398,7 +5398,7 @@
       <c r="I185" s="5"/>
       <c r="J185" s="5"/>
     </row>
-    <row r="186" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>14</v>
       </c>
@@ -5424,7 +5424,7 @@
       <c r="I186" s="5"/>
       <c r="J186" s="5"/>
     </row>
-    <row r="187" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>14</v>
       </c>
@@ -5450,7 +5450,7 @@
       <c r="I187" s="5"/>
       <c r="J187" s="5"/>
     </row>
-    <row r="188" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>14</v>
       </c>
@@ -5476,7 +5476,7 @@
       <c r="I188" s="5"/>
       <c r="J188" s="5"/>
     </row>
-    <row r="189" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>14</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="I189" s="5"/>
       <c r="J189" s="5"/>
     </row>
-    <row r="190" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>14</v>
       </c>
@@ -5528,7 +5528,7 @@
       <c r="I190" s="5"/>
       <c r="J190" s="5"/>
     </row>
-    <row r="191" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>14</v>
       </c>
@@ -5554,7 +5554,7 @@
       <c r="I191" s="5"/>
       <c r="J191" s="5"/>
     </row>
-    <row r="192" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>14</v>
       </c>
@@ -5580,7 +5580,7 @@
       <c r="I192" s="5"/>
       <c r="J192" s="5"/>
     </row>
-    <row r="193" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>14</v>
       </c>
@@ -5606,7 +5606,7 @@
       <c r="I193" s="5"/>
       <c r="J193" s="5"/>
     </row>
-    <row r="194" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>14</v>
       </c>
@@ -5632,7 +5632,7 @@
       <c r="I194" s="5"/>
       <c r="J194" s="5"/>
     </row>
-    <row r="195" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>14</v>
       </c>
@@ -5658,7 +5658,7 @@
       <c r="I195" s="5"/>
       <c r="J195" s="5"/>
     </row>
-    <row r="196" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>14</v>
       </c>
@@ -5684,7 +5684,7 @@
       <c r="I196" s="5"/>
       <c r="J196" s="5"/>
     </row>
-    <row r="197" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>14</v>
       </c>
@@ -5710,7 +5710,7 @@
       <c r="I197" s="5"/>
       <c r="J197" s="5"/>
     </row>
-    <row r="198" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>14</v>
       </c>
@@ -5736,7 +5736,7 @@
       <c r="I198" s="5"/>
       <c r="J198" s="5"/>
     </row>
-    <row r="199" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>14</v>
       </c>
@@ -5762,7 +5762,7 @@
       <c r="I199" s="5"/>
       <c r="J199" s="5"/>
     </row>
-    <row r="200" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>14</v>
       </c>
@@ -5788,7 +5788,7 @@
       <c r="I200" s="5"/>
       <c r="J200" s="5"/>
     </row>
-    <row r="201" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>14</v>
       </c>
@@ -5814,7 +5814,7 @@
       <c r="I201" s="5"/>
       <c r="J201" s="5"/>
     </row>
-    <row r="202" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>14</v>
       </c>
@@ -5840,7 +5840,7 @@
       <c r="I202" s="5"/>
       <c r="J202" s="5"/>
     </row>
-    <row r="203" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>16</v>
       </c>
@@ -5866,7 +5866,7 @@
       <c r="I203" s="5"/>
       <c r="J203" s="5"/>
     </row>
-    <row r="204" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>16</v>
       </c>
@@ -5892,7 +5892,7 @@
       <c r="I204" s="5"/>
       <c r="J204" s="5"/>
     </row>
-    <row r="205" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>16</v>
       </c>
@@ -5918,7 +5918,7 @@
       <c r="I205" s="5"/>
       <c r="J205" s="5"/>
     </row>
-    <row r="206" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>16</v>
       </c>
@@ -5944,7 +5944,7 @@
       <c r="I206" s="5"/>
       <c r="J206" s="5"/>
     </row>
-    <row r="207" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>16</v>
       </c>
@@ -5970,7 +5970,7 @@
       <c r="I207" s="5"/>
       <c r="J207" s="5"/>
     </row>
-    <row r="208" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>16</v>
       </c>
@@ -5996,7 +5996,7 @@
       <c r="I208" s="5"/>
       <c r="J208" s="5"/>
     </row>
-    <row r="209" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>16</v>
       </c>
@@ -6022,7 +6022,7 @@
       <c r="I209" s="5"/>
       <c r="J209" s="5"/>
     </row>
-    <row r="210" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>16</v>
       </c>
@@ -6048,7 +6048,7 @@
       <c r="I210" s="5"/>
       <c r="J210" s="5"/>
     </row>
-    <row r="211" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>16</v>
       </c>
@@ -6074,7 +6074,7 @@
       <c r="I211" s="5"/>
       <c r="J211" s="5"/>
     </row>
-    <row r="212" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>16</v>
       </c>
@@ -6100,7 +6100,7 @@
       <c r="I212" s="5"/>
       <c r="J212" s="5"/>
     </row>
-    <row r="213" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>16</v>
       </c>
@@ -6126,7 +6126,7 @@
       <c r="I213" s="5"/>
       <c r="J213" s="5"/>
     </row>
-    <row r="214" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>16</v>
       </c>
@@ -6152,7 +6152,7 @@
       <c r="I214" s="5"/>
       <c r="J214" s="5"/>
     </row>
-    <row r="215" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>16</v>
       </c>
@@ -6178,7 +6178,7 @@
       <c r="I215" s="5"/>
       <c r="J215" s="5"/>
     </row>
-    <row r="216" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>16</v>
       </c>
@@ -6204,7 +6204,7 @@
       <c r="I216" s="5"/>
       <c r="J216" s="5"/>
     </row>
-    <row r="217" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>16</v>
       </c>
@@ -6230,7 +6230,7 @@
       <c r="I217" s="5"/>
       <c r="J217" s="5"/>
     </row>
-    <row r="218" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>16</v>
       </c>
@@ -6256,7 +6256,7 @@
       <c r="I218" s="5"/>
       <c r="J218" s="5"/>
     </row>
-    <row r="219" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>16</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="I219" s="5"/>
       <c r="J219" s="5"/>
     </row>
-    <row r="220" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>16</v>
       </c>
@@ -6308,7 +6308,7 @@
       <c r="I220" s="5"/>
       <c r="J220" s="5"/>
     </row>
-    <row r="221" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>16</v>
       </c>
@@ -6334,7 +6334,7 @@
       <c r="I221" s="5"/>
       <c r="J221" s="5"/>
     </row>
-    <row r="222" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>16</v>
       </c>
@@ -6360,7 +6360,7 @@
       <c r="I222" s="5"/>
       <c r="J222" s="5"/>
     </row>
-    <row r="223" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>32</v>
       </c>
@@ -6386,7 +6386,7 @@
       <c r="I223" s="5"/>
       <c r="J223" s="5"/>
     </row>
-    <row r="224" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>33</v>
       </c>
@@ -6412,7 +6412,7 @@
       <c r="I224" s="5"/>
       <c r="J224" s="5"/>
     </row>
-    <row r="225" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>33</v>
       </c>
@@ -6438,7 +6438,7 @@
       <c r="I225" s="5"/>
       <c r="J225" s="5"/>
     </row>
-    <row r="226" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>33</v>
       </c>
@@ -6464,7 +6464,7 @@
       <c r="I226" s="5"/>
       <c r="J226" s="5"/>
     </row>
-    <row r="227" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>33</v>
       </c>
@@ -6490,7 +6490,7 @@
       <c r="I227" s="5"/>
       <c r="J227" s="5"/>
     </row>
-    <row r="228" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>33</v>
       </c>
@@ -6516,7 +6516,7 @@
       <c r="I228" s="5"/>
       <c r="J228" s="5"/>
     </row>
-    <row r="229" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>33</v>
       </c>
@@ -6542,7 +6542,7 @@
       <c r="I229" s="5"/>
       <c r="J229" s="5"/>
     </row>
-    <row r="230" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>33</v>
       </c>
@@ -6568,7 +6568,7 @@
       <c r="I230" s="5"/>
       <c r="J230" s="5"/>
     </row>
-    <row r="231" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>33</v>
       </c>
@@ -6594,7 +6594,7 @@
       <c r="I231" s="5"/>
       <c r="J231" s="5"/>
     </row>
-    <row r="232" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>33</v>
       </c>
@@ -6620,7 +6620,7 @@
       <c r="I232" s="5"/>
       <c r="J232" s="5"/>
     </row>
-    <row r="233" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>33</v>
       </c>
@@ -6646,7 +6646,7 @@
       <c r="I233" s="5"/>
       <c r="J233" s="5"/>
     </row>
-    <row r="234" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>32</v>
       </c>
@@ -6672,7 +6672,7 @@
       <c r="I234" s="5"/>
       <c r="J234" s="5"/>
     </row>
-    <row r="235" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>32</v>
       </c>
@@ -6698,7 +6698,7 @@
       <c r="I235" s="5"/>
       <c r="J235" s="5"/>
     </row>
-    <row r="236" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>32</v>
       </c>
@@ -6724,7 +6724,7 @@
       <c r="I236" s="5"/>
       <c r="J236" s="5"/>
     </row>
-    <row r="237" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>32</v>
       </c>
@@ -6750,7 +6750,7 @@
       <c r="I237" s="5"/>
       <c r="J237" s="5"/>
     </row>
-    <row r="238" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>32</v>
       </c>
@@ -6776,7 +6776,7 @@
       <c r="I238" s="5"/>
       <c r="J238" s="5"/>
     </row>
-    <row r="239" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>32</v>
       </c>
@@ -6802,7 +6802,7 @@
       <c r="I239" s="5"/>
       <c r="J239" s="5"/>
     </row>
-    <row r="240" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>32</v>
       </c>
@@ -6828,7 +6828,7 @@
       <c r="I240" s="5"/>
       <c r="J240" s="5"/>
     </row>
-    <row r="241" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>32</v>
       </c>
@@ -6854,7 +6854,7 @@
       <c r="I241" s="5"/>
       <c r="J241" s="5"/>
     </row>
-    <row r="242" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>32</v>
       </c>
@@ -6880,7 +6880,7 @@
       <c r="I242" s="5"/>
       <c r="J242" s="5"/>
     </row>
-    <row r="243" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>32</v>
       </c>
@@ -6906,7 +6906,7 @@
       <c r="I243" s="5"/>
       <c r="J243" s="5"/>
     </row>
-    <row r="244" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>32</v>
       </c>
@@ -6932,7 +6932,7 @@
       <c r="I244" s="5"/>
       <c r="J244" s="5"/>
     </row>
-    <row r="245" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>33</v>
       </c>
@@ -6958,7 +6958,7 @@
       <c r="I245" s="5"/>
       <c r="J245" s="5"/>
     </row>
-    <row r="246" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>33</v>
       </c>
@@ -6984,7 +6984,7 @@
       <c r="I246" s="5"/>
       <c r="J246" s="5"/>
     </row>
-    <row r="247" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>33</v>
       </c>
@@ -7010,7 +7010,7 @@
       <c r="I247" s="5"/>
       <c r="J247" s="5"/>
     </row>
-    <row r="248" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>33</v>
       </c>
@@ -7036,7 +7036,7 @@
       <c r="I248" s="5"/>
       <c r="J248" s="5"/>
     </row>
-    <row r="249" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>33</v>
       </c>
@@ -7062,7 +7062,7 @@
       <c r="I249" s="5"/>
       <c r="J249" s="5"/>
     </row>
-    <row r="250" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>28</v>
       </c>
@@ -7088,7 +7088,7 @@
       <c r="I250" s="5"/>
       <c r="J250" s="5"/>
     </row>
-    <row r="251" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>28</v>
       </c>
@@ -7114,7 +7114,7 @@
       <c r="I251" s="5"/>
       <c r="J251" s="5"/>
     </row>
-    <row r="252" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>28</v>
       </c>
@@ -7140,7 +7140,7 @@
       <c r="I252" s="5"/>
       <c r="J252" s="5"/>
     </row>
-    <row r="253" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>32</v>
       </c>
@@ -7166,7 +7166,7 @@
       <c r="I253" s="5"/>
       <c r="J253" s="5"/>
     </row>
-    <row r="254" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>32</v>
       </c>
@@ -7192,7 +7192,7 @@
       <c r="I254" s="5"/>
       <c r="J254" s="5"/>
     </row>
-    <row r="255" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>32</v>
       </c>
@@ -7218,7 +7218,7 @@
       <c r="I255" s="5"/>
       <c r="J255" s="5"/>
     </row>
-    <row r="256" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>31</v>
       </c>
@@ -7244,7 +7244,7 @@
       <c r="I256" s="5"/>
       <c r="J256" s="5"/>
     </row>
-    <row r="257" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>31</v>
       </c>
@@ -7270,85 +7270,85 @@
       <c r="I257" s="5"/>
       <c r="J257" s="5"/>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G258" s="5"/>
       <c r="H258" s="5"/>
       <c r="I258" s="5"/>
       <c r="J258" s="5"/>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G259" s="5"/>
       <c r="H259" s="5"/>
       <c r="I259" s="5"/>
       <c r="J259" s="5"/>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G260" s="5"/>
       <c r="H260" s="5"/>
       <c r="I260" s="5"/>
       <c r="J260" s="5"/>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G261" s="5"/>
       <c r="H261" s="5"/>
       <c r="I261" s="5"/>
       <c r="J261" s="5"/>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G262" s="5"/>
       <c r="H262" s="5"/>
       <c r="I262" s="5"/>
       <c r="J262" s="5"/>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G263" s="5"/>
       <c r="H263" s="5"/>
       <c r="I263" s="5"/>
       <c r="J263" s="5"/>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G264" s="5"/>
       <c r="H264" s="5"/>
       <c r="I264" s="5"/>
       <c r="J264" s="5"/>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G265" s="5"/>
       <c r="H265" s="5"/>
       <c r="I265" s="5"/>
       <c r="J265" s="5"/>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G266" s="5"/>
       <c r="H266" s="5"/>
       <c r="I266" s="5"/>
       <c r="J266" s="5"/>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G267" s="5"/>
       <c r="H267" s="5"/>
       <c r="I267" s="5"/>
       <c r="J267" s="5"/>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G268" s="5"/>
       <c r="H268" s="5"/>
       <c r="I268" s="5"/>
       <c r="J268" s="5"/>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G269" s="5"/>
       <c r="H269" s="5"/>
       <c r="I269" s="5"/>
       <c r="J269" s="5"/>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G270" s="5"/>
       <c r="H270" s="5"/>
       <c r="I270" s="5"/>
       <c r="J270" s="5"/>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G271" s="5"/>
       <c r="H271" s="5"/>
       <c r="I271" s="5"/>

</xml_diff>

<commit_message>
add db handler on retrieve
</commit_message>
<xml_diff>
--- a/project_db_test_publish.xlsx
+++ b/project_db_test_publish.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dvir levi\PycharmProjects\CDSS-Mini-Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4702486-483C-466E-A250-93A493EB13A4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA983E73-E3F3-41D0-86C2-7B682F036E58}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
   <dimension ref="A1:J271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>